<commit_message>
20250121: Cambio en cantidad = 0
</commit_message>
<xml_diff>
--- a/Nevasa/MBI/20250121/20250121_informe_operaciones_mbi.xlsx
+++ b/Nevasa/MBI/20250121/20250121_informe_operaciones_mbi.xlsx
@@ -16,14 +16,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +48,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +429,399 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>nombre_fondo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_pago</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>fecha_ingreso</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>monto</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>comision</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>nemotecnico</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>compra/venta/vencimiento</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>tipo_operacion</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>precio_factura</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad_factura</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E2" t="n">
+        <v>176126896</v>
+      </c>
+      <c r="F2" t="n">
+        <v>174076278</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>SMT_24032025_21012025_0.57_CFIMBIDT-B</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>15909</v>
+      </c>
+      <c r="L2" t="n">
+        <v>10942</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E3" t="n">
+        <v>183128353</v>
+      </c>
+      <c r="F3" t="n">
+        <v>181918595</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>SMT_25022025_21012025_0.57_BCI</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>29177</v>
+      </c>
+      <c r="L3" t="n">
+        <v>6235</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E4" t="n">
+        <v>334843162</v>
+      </c>
+      <c r="F4" t="n">
+        <v>330944625</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>SMT_24032025_21012025_0.57_CFIMBIDA-A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>17625</v>
+      </c>
+      <c r="L4" t="n">
+        <v>18777</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E5" t="n">
+        <v>72769944.848</v>
+      </c>
+      <c r="F5" t="n">
+        <v>47499964</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>SMT_18022025_21012025_0.57_ENELAM</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>91.38</v>
+      </c>
+      <c r="L5" t="n">
+        <v>519807</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E6" t="n">
+        <v>216637340.952</v>
+      </c>
+      <c r="F6" t="n">
+        <v>141408186</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>SMT_18022025_21012025_0.57_MALLPLAZA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>1654.4</v>
+      </c>
+      <c r="L6" t="n">
+        <v>85474</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E7" t="n">
+        <v>72769906.54800001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>47499939</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>SMT_18022025_21012025_0.57_CHILE</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>123.09</v>
+      </c>
+      <c r="L7" t="n">
+        <v>385896</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E8" t="n">
+        <v>124689480</v>
+      </c>
+      <c r="F8" t="n">
+        <v>81390000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>SMT_18022025_21012025_0.57_RIPLEY</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>SIMULTANEA</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>271.3</v>
+      </c>
+      <c r="L8" t="n">
+        <v>300000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20250121: Cambio cantidad = 0
</commit_message>
<xml_diff>
--- a/Nevasa/MBI/20250121/20250121_informe_operaciones_mbi.xlsx
+++ b/Nevasa/MBI/20250121/20250121_informe_operaciones_mbi.xlsx
@@ -653,7 +653,7 @@
         <v>0.57</v>
       </c>
       <c r="E5" t="n">
-        <v>72769944.848</v>
+        <v>47752663.80848</v>
       </c>
       <c r="F5" t="n">
         <v>47499964</v>
@@ -699,7 +699,7 @@
         <v>0.57</v>
       </c>
       <c r="E6" t="n">
-        <v>216637340.952</v>
+        <v>142160477.54952</v>
       </c>
       <c r="F6" t="n">
         <v>141408186</v>
@@ -745,7 +745,7 @@
         <v>0.57</v>
       </c>
       <c r="E7" t="n">
-        <v>72769906.54800001</v>
+        <v>47752638.67548</v>
       </c>
       <c r="F7" t="n">
         <v>47499939</v>
@@ -791,7 +791,7 @@
         <v>0.57</v>
       </c>
       <c r="E8" t="n">
-        <v>124689480</v>
+        <v>81822994.8</v>
       </c>
       <c r="F8" t="n">
         <v>81390000</v>

</xml_diff>